<commit_message>
updatet optimization project Schedule
</commit_message>
<xml_diff>
--- a/Robust Optimization Project Schedule.xlsx
+++ b/Robust Optimization Project Schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annkathrin\Documents\Meine Dateien\Lehrveranstaltungen\Mathe\Fallstudien\Optimalsteuerung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Texte, Tabellen und Präsentationen\Studium\10. Semester\Fallstudien Nichtlineare Optmierung\Optimalsteuerung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="823" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="823" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Some Hints and Explanations" sheetId="3" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="391">
   <si>
     <t>some hints and explanations concerning this template</t>
   </si>
@@ -1221,6 +1221,12 @@
   <si>
     <t>Implemented Changes</t>
   </si>
+  <si>
+    <t>Präsentation überarbeiten</t>
+  </si>
+  <si>
+    <t>26.5.</t>
+  </si>
 </sst>
 </file>
 
@@ -1633,7 +1639,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,7 +1651,7 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1651,13 +1660,10 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1713,6 +1719,9 @@
           <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <fill>
@@ -1893,9 +1902,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1978,7 +1984,7 @@
   <autoFilter ref="A3:D37"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Task"/>
-    <tableColumn id="2" name="Time Spent (hours)" dataDxfId="23"/>
+    <tableColumn id="2" name="Time Spent (hours)" dataDxfId="5"/>
     <tableColumn id="3" name="When"/>
     <tableColumn id="4" name="Notes"/>
   </tableColumns>
@@ -1987,8 +1993,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:D26" totalsRowShown="0">
-  <autoFilter ref="A3:D26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:D27" totalsRowShown="0">
+  <autoFilter ref="A3:D27"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Task"/>
     <tableColumn id="2" name="Time Spent (hours)"/>
@@ -2381,7 +2387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
@@ -11023,17 +11029,17 @@
     <sortCondition ref="E40:E49"/>
   </sortState>
   <conditionalFormatting sqref="A15:B304">
-    <cfRule type="expression" dxfId="22" priority="79">
+    <cfRule type="expression" dxfId="23" priority="79">
       <formula>(MID($A15,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD302">
-    <cfRule type="expression" dxfId="21" priority="83">
+    <cfRule type="expression" dxfId="22" priority="83">
       <formula>(MID($A3,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B302">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>(MID($A3,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11090,385 +11096,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
-      <c r="AJ1" s="59"/>
-      <c r="AK1" s="59"/>
-      <c r="AL1" s="59"/>
-      <c r="AM1" s="59"/>
-      <c r="AN1" s="59"/>
-      <c r="AO1" s="59"/>
-      <c r="AP1" s="59"/>
-      <c r="AQ1" s="59"/>
-      <c r="AR1" s="59"/>
-      <c r="AS1" s="59"/>
-      <c r="AT1" s="59"/>
-      <c r="AU1" s="59"/>
-      <c r="AV1" s="59"/>
-      <c r="AW1" s="59"/>
-      <c r="AX1" s="59"/>
-      <c r="AY1" s="59"/>
-      <c r="AZ1" s="59"/>
-      <c r="BA1" s="59"/>
-      <c r="BB1" s="59"/>
-      <c r="BC1" s="59"/>
-      <c r="BD1" s="59"/>
-      <c r="BE1" s="59"/>
-      <c r="BF1" s="59"/>
-      <c r="BG1" s="59"/>
-      <c r="BH1" s="59"/>
-      <c r="BI1" s="59"/>
-      <c r="BJ1" s="59"/>
-      <c r="BK1" s="59"/>
-      <c r="BL1" s="59"/>
-      <c r="BM1" s="59"/>
-      <c r="BN1" s="59"/>
-      <c r="BO1" s="59"/>
-      <c r="BP1" s="59"/>
-      <c r="BQ1" s="59"/>
-      <c r="BR1" s="59"/>
-      <c r="BS1" s="59"/>
-      <c r="BT1" s="59"/>
-      <c r="BU1" s="59"/>
-      <c r="BV1" s="59"/>
-      <c r="BW1" s="59"/>
-      <c r="BX1" s="59"/>
-      <c r="BY1" s="59"/>
-      <c r="BZ1" s="59"/>
-      <c r="CA1" s="59"/>
-      <c r="CB1" s="59"/>
-      <c r="CC1" s="59"/>
-      <c r="CD1" s="59"/>
-      <c r="CE1" s="59"/>
-      <c r="CF1" s="59"/>
-      <c r="CG1" s="59"/>
-      <c r="CH1" s="59"/>
-      <c r="CI1" s="59"/>
-      <c r="CJ1" s="59"/>
-      <c r="CK1" s="59"/>
-      <c r="CL1" s="59"/>
-      <c r="CM1" s="59"/>
-      <c r="CN1" s="59"/>
-      <c r="CO1" s="59"/>
-      <c r="CP1" s="59"/>
-      <c r="CQ1" s="59"/>
-      <c r="CR1" s="59"/>
-      <c r="CS1" s="59"/>
-      <c r="CT1" s="59"/>
-      <c r="CU1" s="59"/>
-      <c r="CV1" s="59"/>
-      <c r="CW1" s="59"/>
-      <c r="CX1" s="59"/>
-      <c r="CY1" s="59"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="53"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="53"/>
+      <c r="BB1" s="53"/>
+      <c r="BC1" s="53"/>
+      <c r="BD1" s="53"/>
+      <c r="BE1" s="53"/>
+      <c r="BF1" s="53"/>
+      <c r="BG1" s="53"/>
+      <c r="BH1" s="53"/>
+      <c r="BI1" s="53"/>
+      <c r="BJ1" s="53"/>
+      <c r="BK1" s="53"/>
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="53"/>
+      <c r="BQ1" s="53"/>
+      <c r="BR1" s="53"/>
+      <c r="BS1" s="53"/>
+      <c r="BT1" s="53"/>
+      <c r="BU1" s="53"/>
+      <c r="BV1" s="53"/>
+      <c r="BW1" s="53"/>
+      <c r="BX1" s="53"/>
+      <c r="BY1" s="53"/>
+      <c r="BZ1" s="53"/>
+      <c r="CA1" s="53"/>
+      <c r="CB1" s="53"/>
+      <c r="CC1" s="53"/>
+      <c r="CD1" s="53"/>
+      <c r="CE1" s="53"/>
+      <c r="CF1" s="53"/>
+      <c r="CG1" s="53"/>
+      <c r="CH1" s="53"/>
+      <c r="CI1" s="53"/>
+      <c r="CJ1" s="53"/>
+      <c r="CK1" s="53"/>
+      <c r="CL1" s="53"/>
+      <c r="CM1" s="53"/>
+      <c r="CN1" s="53"/>
+      <c r="CO1" s="53"/>
+      <c r="CP1" s="53"/>
+      <c r="CQ1" s="53"/>
+      <c r="CR1" s="53"/>
+      <c r="CS1" s="53"/>
+      <c r="CT1" s="53"/>
+      <c r="CU1" s="53"/>
+      <c r="CV1" s="53"/>
+      <c r="CW1" s="53"/>
+      <c r="CX1" s="53"/>
+      <c r="CY1" s="53"/>
       <c r="CZ1" s="11"/>
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="53" t="s">
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53" t="s">
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="53" t="s">
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="53" t="s">
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="56"/>
+      <c r="AI2" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="55"/>
-      <c r="AP2" s="53" t="s">
+      <c r="AJ2" s="55"/>
+      <c r="AK2" s="55"/>
+      <c r="AL2" s="55"/>
+      <c r="AM2" s="55"/>
+      <c r="AN2" s="55"/>
+      <c r="AO2" s="56"/>
+      <c r="AP2" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="55"/>
-      <c r="AW2" s="53" t="s">
+      <c r="AQ2" s="55"/>
+      <c r="AR2" s="55"/>
+      <c r="AS2" s="55"/>
+      <c r="AT2" s="55"/>
+      <c r="AU2" s="55"/>
+      <c r="AV2" s="56"/>
+      <c r="AW2" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="AX2" s="54"/>
-      <c r="AY2" s="54"/>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="54"/>
-      <c r="BB2" s="54"/>
-      <c r="BC2" s="55"/>
-      <c r="BD2" s="53" t="s">
+      <c r="AX2" s="55"/>
+      <c r="AY2" s="55"/>
+      <c r="AZ2" s="55"/>
+      <c r="BA2" s="55"/>
+      <c r="BB2" s="55"/>
+      <c r="BC2" s="56"/>
+      <c r="BD2" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="BE2" s="54"/>
-      <c r="BF2" s="54"/>
-      <c r="BG2" s="54"/>
-      <c r="BH2" s="54"/>
-      <c r="BI2" s="54"/>
-      <c r="BJ2" s="55"/>
-      <c r="BK2" s="53" t="s">
+      <c r="BE2" s="55"/>
+      <c r="BF2" s="55"/>
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="55"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="BL2" s="54"/>
-      <c r="BM2" s="54"/>
-      <c r="BN2" s="54"/>
-      <c r="BO2" s="54"/>
-      <c r="BP2" s="54"/>
-      <c r="BQ2" s="55"/>
-      <c r="BR2" s="53" t="s">
+      <c r="BL2" s="55"/>
+      <c r="BM2" s="55"/>
+      <c r="BN2" s="55"/>
+      <c r="BO2" s="55"/>
+      <c r="BP2" s="55"/>
+      <c r="BQ2" s="56"/>
+      <c r="BR2" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="BS2" s="54"/>
-      <c r="BT2" s="54"/>
-      <c r="BU2" s="54"/>
-      <c r="BV2" s="54"/>
-      <c r="BW2" s="54"/>
-      <c r="BX2" s="55"/>
-      <c r="BY2" s="53" t="s">
+      <c r="BS2" s="55"/>
+      <c r="BT2" s="55"/>
+      <c r="BU2" s="55"/>
+      <c r="BV2" s="55"/>
+      <c r="BW2" s="55"/>
+      <c r="BX2" s="56"/>
+      <c r="BY2" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="BZ2" s="54"/>
-      <c r="CA2" s="54"/>
-      <c r="CB2" s="54"/>
-      <c r="CC2" s="54"/>
-      <c r="CD2" s="54"/>
-      <c r="CE2" s="55"/>
-      <c r="CF2" s="53" t="s">
+      <c r="BZ2" s="55"/>
+      <c r="CA2" s="55"/>
+      <c r="CB2" s="55"/>
+      <c r="CC2" s="55"/>
+      <c r="CD2" s="55"/>
+      <c r="CE2" s="56"/>
+      <c r="CF2" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="CG2" s="54"/>
-      <c r="CH2" s="54"/>
-      <c r="CI2" s="54"/>
-      <c r="CJ2" s="54"/>
-      <c r="CK2" s="54"/>
-      <c r="CL2" s="55"/>
-      <c r="CM2" s="53" t="s">
+      <c r="CG2" s="55"/>
+      <c r="CH2" s="55"/>
+      <c r="CI2" s="55"/>
+      <c r="CJ2" s="55"/>
+      <c r="CK2" s="55"/>
+      <c r="CL2" s="56"/>
+      <c r="CM2" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="CN2" s="54"/>
-      <c r="CO2" s="54"/>
-      <c r="CP2" s="54"/>
-      <c r="CQ2" s="54"/>
-      <c r="CR2" s="54"/>
-      <c r="CS2" s="55"/>
-      <c r="CT2" s="53" t="s">
+      <c r="CN2" s="55"/>
+      <c r="CO2" s="55"/>
+      <c r="CP2" s="55"/>
+      <c r="CQ2" s="55"/>
+      <c r="CR2" s="55"/>
+      <c r="CS2" s="56"/>
+      <c r="CT2" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="CU2" s="54"/>
-      <c r="CV2" s="54"/>
-      <c r="CW2" s="54"/>
-      <c r="CX2" s="54"/>
-      <c r="CY2" s="54"/>
-      <c r="CZ2" s="55"/>
+      <c r="CU2" s="55"/>
+      <c r="CV2" s="55"/>
+      <c r="CW2" s="55"/>
+      <c r="CX2" s="55"/>
+      <c r="CY2" s="55"/>
+      <c r="CZ2" s="56"/>
     </row>
     <row r="3" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="G3" s="61">
+      <c r="G3" s="57">
         <f>G5</f>
         <v>42107</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="56">
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="61">
         <f>N5</f>
         <v>42114</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="56">
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="61">
         <f>U5</f>
         <v>42121</v>
       </c>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="57"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="56">
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="61">
         <f>AB5</f>
         <v>42128</v>
       </c>
-      <c r="AC3" s="57"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="57"/>
-      <c r="AF3" s="57"/>
-      <c r="AG3" s="57"/>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="56">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="61">
         <f>AI5</f>
         <v>42135</v>
       </c>
-      <c r="AJ3" s="57"/>
-      <c r="AK3" s="57"/>
-      <c r="AL3" s="57"/>
-      <c r="AM3" s="57"/>
-      <c r="AN3" s="57"/>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="56">
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="61">
         <f>AP5</f>
         <v>42142</v>
       </c>
-      <c r="AQ3" s="57"/>
-      <c r="AR3" s="57"/>
-      <c r="AS3" s="57"/>
-      <c r="AT3" s="57"/>
-      <c r="AU3" s="57"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="56">
+      <c r="AQ3" s="58"/>
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="59"/>
+      <c r="AW3" s="61">
         <f t="shared" ref="AW3" si="0">AW5</f>
         <v>42149</v>
       </c>
-      <c r="AX3" s="57"/>
-      <c r="AY3" s="57"/>
-      <c r="AZ3" s="57"/>
-      <c r="BA3" s="57"/>
-      <c r="BB3" s="57"/>
-      <c r="BC3" s="58"/>
-      <c r="BD3" s="56">
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
+      <c r="BC3" s="59"/>
+      <c r="BD3" s="61">
         <f t="shared" ref="BD3" si="1">BD5</f>
         <v>42156</v>
       </c>
-      <c r="BE3" s="57"/>
-      <c r="BF3" s="57"/>
-      <c r="BG3" s="57"/>
-      <c r="BH3" s="57"/>
-      <c r="BI3" s="57"/>
-      <c r="BJ3" s="58"/>
-      <c r="BK3" s="56">
+      <c r="BE3" s="58"/>
+      <c r="BF3" s="58"/>
+      <c r="BG3" s="58"/>
+      <c r="BH3" s="58"/>
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="59"/>
+      <c r="BK3" s="61">
         <f t="shared" ref="BK3" si="2">BK5</f>
         <v>42163</v>
       </c>
-      <c r="BL3" s="57"/>
-      <c r="BM3" s="57"/>
-      <c r="BN3" s="57"/>
-      <c r="BO3" s="57"/>
-      <c r="BP3" s="57"/>
-      <c r="BQ3" s="58"/>
-      <c r="BR3" s="56">
+      <c r="BL3" s="58"/>
+      <c r="BM3" s="58"/>
+      <c r="BN3" s="58"/>
+      <c r="BO3" s="58"/>
+      <c r="BP3" s="58"/>
+      <c r="BQ3" s="59"/>
+      <c r="BR3" s="61">
         <f t="shared" ref="BR3" si="3">BR5</f>
         <v>42170</v>
       </c>
-      <c r="BS3" s="57"/>
-      <c r="BT3" s="57"/>
-      <c r="BU3" s="57"/>
-      <c r="BV3" s="57"/>
-      <c r="BW3" s="57"/>
-      <c r="BX3" s="58"/>
-      <c r="BY3" s="56">
+      <c r="BS3" s="58"/>
+      <c r="BT3" s="58"/>
+      <c r="BU3" s="58"/>
+      <c r="BV3" s="58"/>
+      <c r="BW3" s="58"/>
+      <c r="BX3" s="59"/>
+      <c r="BY3" s="61">
         <f t="shared" ref="BY3" si="4">BY5</f>
         <v>42177</v>
       </c>
-      <c r="BZ3" s="57"/>
-      <c r="CA3" s="57"/>
-      <c r="CB3" s="57"/>
-      <c r="CC3" s="57"/>
-      <c r="CD3" s="57"/>
-      <c r="CE3" s="58"/>
-      <c r="CF3" s="56">
+      <c r="BZ3" s="58"/>
+      <c r="CA3" s="58"/>
+      <c r="CB3" s="58"/>
+      <c r="CC3" s="58"/>
+      <c r="CD3" s="58"/>
+      <c r="CE3" s="59"/>
+      <c r="CF3" s="61">
         <f t="shared" ref="CF3" si="5">CF5</f>
         <v>42184</v>
       </c>
-      <c r="CG3" s="57"/>
-      <c r="CH3" s="57"/>
-      <c r="CI3" s="57"/>
-      <c r="CJ3" s="57"/>
-      <c r="CK3" s="57"/>
-      <c r="CL3" s="58"/>
-      <c r="CM3" s="56">
+      <c r="CG3" s="58"/>
+      <c r="CH3" s="58"/>
+      <c r="CI3" s="58"/>
+      <c r="CJ3" s="58"/>
+      <c r="CK3" s="58"/>
+      <c r="CL3" s="59"/>
+      <c r="CM3" s="61">
         <f t="shared" ref="CM3" si="6">CM5</f>
         <v>42191</v>
       </c>
-      <c r="CN3" s="57"/>
-      <c r="CO3" s="57"/>
-      <c r="CP3" s="57"/>
-      <c r="CQ3" s="57"/>
-      <c r="CR3" s="57"/>
-      <c r="CS3" s="58"/>
-      <c r="CT3" s="56">
+      <c r="CN3" s="58"/>
+      <c r="CO3" s="58"/>
+      <c r="CP3" s="58"/>
+      <c r="CQ3" s="58"/>
+      <c r="CR3" s="58"/>
+      <c r="CS3" s="59"/>
+      <c r="CT3" s="61">
         <f t="shared" ref="CT3" si="7">CT5</f>
         <v>42198</v>
       </c>
-      <c r="CU3" s="57"/>
-      <c r="CV3" s="57"/>
-      <c r="CW3" s="57"/>
-      <c r="CX3" s="57"/>
-      <c r="CY3" s="57"/>
-      <c r="CZ3" s="58"/>
+      <c r="CU3" s="58"/>
+      <c r="CV3" s="58"/>
+      <c r="CW3" s="58"/>
+      <c r="CX3" s="58"/>
+      <c r="CY3" s="58"/>
+      <c r="CZ3" s="59"/>
     </row>
     <row r="4" spans="1:104" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -23989,6 +23995,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="CM3:CS3"/>
+    <mergeCell ref="CT3:CZ3"/>
+    <mergeCell ref="BY2:CE2"/>
+    <mergeCell ref="CF2:CL2"/>
+    <mergeCell ref="BY3:CE3"/>
+    <mergeCell ref="CF3:CL3"/>
+    <mergeCell ref="CM2:CS2"/>
+    <mergeCell ref="BD3:BJ3"/>
+    <mergeCell ref="BK2:BQ2"/>
+    <mergeCell ref="BR2:BX2"/>
+    <mergeCell ref="BK3:BQ3"/>
+    <mergeCell ref="BR3:BX3"/>
     <mergeCell ref="A1:CY1"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="G3:M3"/>
@@ -24005,22 +24024,9 @@
     <mergeCell ref="AI3:AO3"/>
     <mergeCell ref="AP3:AV3"/>
     <mergeCell ref="AW3:BC3"/>
-    <mergeCell ref="BD3:BJ3"/>
-    <mergeCell ref="BK2:BQ2"/>
-    <mergeCell ref="BR2:BX2"/>
-    <mergeCell ref="BK3:BQ3"/>
-    <mergeCell ref="BR3:BX3"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="CM3:CS3"/>
-    <mergeCell ref="CT3:CZ3"/>
-    <mergeCell ref="BY2:CE2"/>
-    <mergeCell ref="CF2:CL2"/>
-    <mergeCell ref="BY3:CE3"/>
-    <mergeCell ref="CF3:CL3"/>
-    <mergeCell ref="CM2:CS2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:CW300">
-    <cfRule type="expression" dxfId="19" priority="77">
+    <cfRule type="expression" dxfId="20" priority="77">
       <formula>NOT(ISNA(VLOOKUP(G$5,$F:$F,1,FALSE)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47036,7 +47042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -47594,7 +47600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -47965,7 +47971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -48451,10 +48457,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48493,7 +48499,7 @@
       </c>
       <c r="H3">
         <f>SUM(Table13[Time Spent (hours)])</f>
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -48727,6 +48733,17 @@
       </c>
       <c r="C26" t="s">
         <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>389</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -48742,7 +48759,7 @@
           <x14:formula1>
             <xm:f>'task extraction'!$D$2:$D$350</xm:f>
           </x14:formula1>
-          <xm:sqref>A4:A26</xm:sqref>
+          <xm:sqref>A4:A27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -48754,7 +48771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>